<commit_message>
Fixed a couple mistakes
</commit_message>
<xml_diff>
--- a/prelab/state_transition_table.xlsx
+++ b/prelab/state_transition_table.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\col.missouri.edu\files\MUENGRECEPL\s\zrrm74\Desktop\lab04\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11988"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="24">
   <si>
     <t>Input</t>
   </si>
@@ -87,17 +82,34 @@
   </si>
   <si>
     <t>$0.00 = 00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"case </t>
+  </si>
+  <si>
+    <t>&lt;-$0.20</t>
+  </si>
+  <si>
+    <t>&lt;-$0.25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -125,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -140,6 +152,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -200,7 +217,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -235,7 +252,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -412,26 +429,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16">
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -448,7 +465,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16">
       <c r="D4" t="s">
         <v>1</v>
       </c>
@@ -468,7 +485,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16">
       <c r="B5" s="1">
         <v>0</v>
       </c>
@@ -497,7 +514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16">
       <c r="B6" s="1">
         <v>0</v>
       </c>
@@ -526,7 +543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16">
       <c r="B7" s="1">
         <v>0</v>
       </c>
@@ -555,7 +572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16">
       <c r="B8" s="1">
         <v>0</v>
       </c>
@@ -584,7 +601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16">
       <c r="B10" s="1">
         <v>0.05</v>
       </c>
@@ -613,7 +630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16">
       <c r="B11" s="1">
         <v>0.05</v>
       </c>
@@ -642,7 +659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16">
       <c r="B12" s="1">
         <v>0.05</v>
       </c>
@@ -671,7 +688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16">
       <c r="B13" s="1">
         <v>0.05</v>
       </c>
@@ -700,7 +717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16">
       <c r="B15" s="1">
         <v>0.1</v>
       </c>
@@ -729,7 +746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16">
       <c r="B16" s="1">
         <v>0.1</v>
       </c>
@@ -758,7 +775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:16">
       <c r="B17" s="1">
         <v>0.1</v>
       </c>
@@ -768,8 +785,11 @@
       <c r="E17">
         <v>0</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>8</v>
+      <c r="F17" s="6">
+        <v>0</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -787,7 +807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:16">
       <c r="B18" s="1">
         <v>0.1</v>
       </c>
@@ -800,6 +820,7 @@
       <c r="F18" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="G18" s="7"/>
       <c r="H18" s="2" t="s">
         <v>8</v>
       </c>
@@ -816,7 +837,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:16">
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" spans="2:16">
       <c r="B20" s="1">
         <v>0.15</v>
       </c>
@@ -826,9 +850,10 @@
       <c r="E20">
         <v>0</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="8">
         <v>0.15</v>
       </c>
+      <c r="G20" s="7"/>
       <c r="H20">
         <v>0</v>
       </c>
@@ -845,7 +870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:16">
       <c r="B21" s="1">
         <v>0.15</v>
       </c>
@@ -855,8 +880,11 @@
       <c r="E21">
         <v>1</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>8</v>
+      <c r="F21" s="6">
+        <v>0</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -874,7 +902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:16">
       <c r="B22" s="1">
         <v>0.15</v>
       </c>
@@ -884,8 +912,11 @@
       <c r="E22">
         <v>0</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>8</v>
+      <c r="F22" s="6">
+        <v>0</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -903,7 +934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:16">
       <c r="B23" s="1">
         <v>0.15</v>
       </c>
@@ -932,19 +963,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:16">
       <c r="B25" s="1"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:16">
       <c r="B26" s="1"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:16">
       <c r="B27" s="1"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:16">
       <c r="B28" s="4" t="s">
         <v>10</v>
       </c>
@@ -956,7 +987,7 @@
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:16">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -965,8 +996,11 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
-    </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="P29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16">
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -979,12 +1013,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:16">
       <c r="N31" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:16">
       <c r="B32" s="5" t="s">
         <v>14</v>
       </c>
@@ -999,7 +1033,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -1012,7 +1046,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:14">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -1028,6 +1062,6 @@
     <mergeCell ref="B32:I34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>